<commit_message>
Improve demo: level display
</commit_message>
<xml_diff>
--- a/demo/Results/Distance/Anova.xlsx
+++ b/demo/Results/Distance/Anova.xlsx
@@ -123,7 +123,7 @@
     <col min="3" max="3" width="4.42578125" customWidth="true"/>
     <col min="4" max="4" width="11.7109375" customWidth="true"/>
     <col min="5" max="5" width="13.7109375" customWidth="true"/>
-    <col min="6" max="6" width="14.7109375" customWidth="true"/>
+    <col min="6" max="6" width="12.7109375" customWidth="true"/>
     <col min="7" max="7" width="10" customWidth="true"/>
     <col min="8" max="8" width="11.5703125" customWidth="true"/>
   </cols>
@@ -165,13 +165,13 @@
         <v>490</v>
       </c>
       <c r="D2" s="0">
-        <v>364511.53239454993</v>
+        <v>375858.88519869605</v>
       </c>
       <c r="E2" s="0">
         <v>0</v>
       </c>
       <c r="F2" s="0">
-        <v>0.99865753988268102</v>
+        <v>0.99869801660302171</v>
       </c>
       <c r="G2" s="0" t="s">
         <v>11</v>
@@ -191,13 +191,13 @@
         <v>490</v>
       </c>
       <c r="D3" s="0">
-        <v>4.0091497522804866</v>
+        <v>4.009086477938423</v>
       </c>
       <c r="E3" s="0">
-        <v>0.045804547246759086</v>
+        <v>0.0458062517406711</v>
       </c>
       <c r="F3" s="0">
-        <v>0.0081155374435693418</v>
+        <v>0.0081154103996778654</v>
       </c>
       <c r="G3" s="0" t="s">
         <v>12</v>
@@ -217,13 +217,13 @@
         <v>490</v>
       </c>
       <c r="D4" s="0">
-        <v>917.33290070225962</v>
+        <v>945.88974503464829</v>
       </c>
       <c r="E4" s="0">
         <v>0</v>
       </c>
       <c r="F4" s="0">
-        <v>0.65182367316539691</v>
+        <v>0.65874817220860071</v>
       </c>
       <c r="G4" s="0" t="s">
         <v>13</v>
@@ -243,13 +243,13 @@
         <v>490</v>
       </c>
       <c r="D5" s="0">
-        <v>138.89339214208266</v>
+        <v>138.89344621813584</v>
       </c>
       <c r="E5" s="0">
         <v>0</v>
       </c>
       <c r="F5" s="0">
-        <v>0.22085363573148051</v>
+        <v>0.22085370272718619</v>
       </c>
       <c r="G5" s="0" t="s">
         <v>14</v>

</xml_diff>